<commit_message>
feat: Add transfer for third parties, made post processing bank orietned instead of astor oriented, fix regex for cuils
</commit_message>
<xml_diff>
--- a/post_process/supervielle.xlsx
+++ b/post_process/supervielle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,131 +448,401 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IMPUESTOS DEBITOS</t>
+          <t>Impuesto Débitos y Créditos/DB</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2523551.29</v>
+        <v>2518822.23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>COMISIONES</t>
+          <t>Devolución Imp. Débitos</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9330.280000000001</v>
+        <v>4729.06</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IVA</t>
+          <t>COMIS.TRANSFERENCIAS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>57780.07999999997</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PERC. IVA</t>
+          <t>IVA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8103.85</v>
+        <v>57780.07999999997</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IIBB</t>
+          <t>Comisión Consulta Cámara</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4150659.69</v>
+        <v>700</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TRANSFERENCIA</t>
+          <t>Comisión Mantenimiento Cuenta</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>695329714.9700006</v>
+        <v>4706</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IMPUESTOS CREDITOS</t>
+          <t>Percepción I.V.A. RG. 3337</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>926362.7000000002</v>
+        <v>8103.85</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CHEQUE / FALLA</t>
+          <t>Cobro Percepción IIBB</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>785580.52</v>
+        <v>536.72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CHEQUE</t>
+          <t>Débito Comisión Pago a Prov.</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>231919492.24</v>
+        <v>784.08</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>OPERACIONES FINANCIERAS</t>
+          <t>Trf. Pago.Prov-Terceros O/Bcos</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>81129382.82000001</v>
+        <v>12187554.96</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INTERESES</t>
+          <t>Impuesto Débitos y Créditos/CR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>533194.0699999999</v>
+        <v>926362.7000000002</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SELLOS</t>
+          <t>IIBB- Acreditaciones Bancarias</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10987.52</v>
+        <v>4150122.97</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SUELDOS</t>
+          <t>Debito Transf. HomeBanking</t>
         </is>
       </c>
       <c r="B14" t="n">
+        <v>20750000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CRED BCA ELECTR INTERBANC EXEN</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>204917000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Transferencia por CBU</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>100501494.83</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CRED BCA ELECTRONICA INTERBANC</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>103929174.48</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Rech. Cheques Falla Técnica</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>785580.52</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Trf. Masivas Pago Proveedores</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>119205508.5099999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Pago Cheque de Cámara Recibida</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>195885949.84</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SIPAP - Pago Cheque de Cámara</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>32240355.95</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SIPAP - Pago Cámara SPV 24 hs.</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1592003.24</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Crédito Transf. HomeBanking</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>14600000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Descto. Docum.- Acreditación</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>76168604.92000002</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Pago Cámara SPV 24 hs.</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2115162.71</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Crédito por Transferencia</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>89556032.45</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Préstamos Inversion Productiva</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>4455000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>DEB BCA ELECTRONICA INTERBANC</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>666200.8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Credito DEBIN</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>7547000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Pago de Servicios</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>14489512.88</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Comisión Riesgo Contigente</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Acreditación Cheque Dep.48 Hs.</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>86020.5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Intereses de Sobregiro</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>530844.48</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>IMPUESTO A LOS SELLOS</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>10987.52</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Débito Automático de Servicio</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1414130.89</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Pago Automático de Préstamo</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>505777.9</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>DEB BCA ELECTRONICA INTRABANC</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>4566105.17</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Deb. Pago de Sueldo</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
         <v>8975093</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>COMISIONES DATANET</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>94.2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>DEB BCA ELECTR INTERBANC EXEN</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Contras.Ints.Sobreg.</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2349.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>